<commit_message>
Deleted reports and logs
</commit_message>
<xml_diff>
--- a/target/test-classes/com/gtpl/testData/RequiredData.xlsx
+++ b/target/test-classes/com/gtpl/testData/RequiredData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\git\GTPLBank\src\test\java\com\gtpl\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59205384-8E85-40E1-9002-F16A20488D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE67E6FD-2687-4C25-8747-478D10F82FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>mngr599593</t>
+    <t>mngr608625</t>
   </si>
   <si>
-    <t>zAdavAq</t>
+    <t>uvabujU</t>
   </si>
 </sst>
 </file>
@@ -103,7 +103,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -391,13 +391,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -405,7 +405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>